<commit_message>
Practice_43_Voice_Recorder: added FFT, new features to VoiceRecognition functions, and better functionality all over
</commit_message>
<xml_diff>
--- a/Practice_43_Voice_Recorder/Math draft.xlsx
+++ b/Practice_43_Voice_Recorder/Math draft.xlsx
@@ -3110,15 +3110,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G1:S25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1">
+        <f>A1/$D$1*$E$1-$F$1</f>
+        <v>9.9999999999999964</v>
+      </c>
+      <c r="D1">
+        <v>18</v>
+      </c>
+      <c r="E1">
+        <v>4.05</v>
+      </c>
+      <c r="F1">
+        <v>12.5</v>
+      </c>
       <c r="G1">
         <v>100</v>
       </c>
@@ -3149,12 +3165,19 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:B17" si="0">A2/$D$1*$E$1-$F$1</f>
+        <v>15.625</v>
+      </c>
       <c r="G2">
         <v>125</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H33" si="0">G2/$K$1*$L$1-$M$1</f>
+        <f t="shared" ref="H2:H24" si="1">G2/$K$1*$L$1-$M$1</f>
         <v>7.9398148148148167</v>
       </c>
       <c r="O2">
@@ -3165,12 +3188,19 @@
         <v>91.38858966835852</v>
       </c>
     </row>
-    <row r="3" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3">
+        <f t="shared" si="0"/>
+        <v>21.25</v>
+      </c>
       <c r="G3">
         <v>150</v>
       </c>
       <c r="H3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11.527777777777779</v>
       </c>
       <c r="O3">
@@ -3181,348 +3211,446 @@
         <v>92.205957846728964</v>
       </c>
     </row>
-    <row r="4" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>175</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>26.874999999999993</v>
+      </c>
       <c r="G4">
         <v>175</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.11574074074074</v>
       </c>
       <c r="O4">
         <v>1000</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q24" si="1">LOG(O4,$R$1)+$S$1</f>
+        <f t="shared" ref="Q4:Q24" si="2">LOG(O4,$R$1)+$S$1</f>
         <v>92.93711859730297</v>
       </c>
     </row>
-    <row r="5" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>200</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>32.499999999999993</v>
+      </c>
       <c r="G5">
         <v>200</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.703703703703702</v>
       </c>
       <c r="O5">
         <v>1100</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>93.598533949799872</v>
       </c>
     </row>
-    <row r="6" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>225</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>38.125</v>
+      </c>
       <c r="G6">
         <v>225</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.291666666666671</v>
       </c>
       <c r="O6">
         <v>1200</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.202358858125393</v>
       </c>
     </row>
-    <row r="7" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>250</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>43.75</v>
+      </c>
       <c r="G7">
         <v>250</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.879629629629633</v>
       </c>
       <c r="O7">
         <v>1300</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>94.757823928272018</v>
       </c>
     </row>
-    <row r="8" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>275</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>49.375</v>
+      </c>
       <c r="G8">
         <v>275</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.467592592592595</v>
       </c>
       <c r="O8">
         <v>1400</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95.27210425620251</v>
       </c>
     </row>
-    <row r="9" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>300</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
       <c r="G9">
         <v>300</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33.055555555555557</v>
       </c>
       <c r="O9">
         <v>1500</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>95.750887787069843</v>
       </c>
     </row>
-    <row r="10" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>325</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>60.625</v>
+      </c>
       <c r="G10">
         <v>325</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36.643518518518519</v>
       </c>
       <c r="O10">
         <v>1600</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96.198759869521808</v>
       </c>
     </row>
-    <row r="11" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>350</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>66.249999999999986</v>
+      </c>
       <c r="G11">
         <v>350</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40.231481481481481</v>
       </c>
       <c r="O11">
         <v>1700</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>96.619471022213276</v>
       </c>
     </row>
-    <row r="12" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>375</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>71.874999999999986</v>
+      </c>
       <c r="G12">
         <v>375</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43.819444444444443</v>
       </c>
       <c r="O12">
         <v>1800</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97.016128047892252</v>
       </c>
     </row>
-    <row r="13" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>400</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>77.499999999999986</v>
+      </c>
       <c r="G13">
         <v>400</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>47.407407407407405</v>
       </c>
       <c r="O13">
         <v>1900</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97.391333406736663</v>
       </c>
     </row>
-    <row r="14" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>425</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>83.125</v>
+      </c>
       <c r="G14">
         <v>425</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50.995370370370367</v>
       </c>
       <c r="O14">
         <v>2000</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>97.747288798466272</v>
       </c>
     </row>
-    <row r="15" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>450</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>88.75</v>
+      </c>
       <c r="G15">
         <v>450</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>54.583333333333343</v>
       </c>
       <c r="O15">
         <v>2100</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>98.085873445969384</v>
       </c>
     </row>
-    <row r="16" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>475</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>94.375</v>
+      </c>
       <c r="G16">
         <v>475</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58.171296296296291</v>
       </c>
       <c r="O16">
         <v>2200</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>98.40870415096316</v>
       </c>
     </row>
-    <row r="17" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>500</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
       <c r="G17">
         <v>500</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61.759259259259267</v>
       </c>
       <c r="O17">
         <v>2300</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>98.717181989010015</v>
       </c>
     </row>
-    <row r="18" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G18">
         <v>525</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65.347222222222214</v>
       </c>
       <c r="O18">
         <v>2400</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.012529059288681</v>
       </c>
     </row>
-    <row r="19" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G19">
         <v>550</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>68.93518518518519</v>
       </c>
       <c r="O19">
         <v>2500</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.295817727410736</v>
       </c>
     </row>
-    <row r="20" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G20">
         <v>575</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72.523148148148152</v>
       </c>
       <c r="O20">
         <v>2600</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.567994129435306</v>
       </c>
     </row>
-    <row r="21" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G21">
         <v>600</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>76.111111111111114</v>
       </c>
       <c r="O21">
         <v>2700</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>99.829897237659111</v>
       </c>
     </row>
-    <row r="22" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G22">
         <v>625</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>79.699074074074076</v>
       </c>
       <c r="O22">
         <v>2800</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.0822744573658</v>
       </c>
     </row>
-    <row r="23" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G23">
         <v>650</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>83.287037037037038</v>
       </c>
       <c r="O23">
         <v>2900</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.32579448544888</v>
       </c>
     </row>
-    <row r="24" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G24">
         <v>675</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>86.875</v>
       </c>
       <c r="O24">
         <v>3000</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.56105798823313</v>
       </c>
     </row>
-    <row r="25" spans="7:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G25">
         <v>700</v>
       </c>
       <c r="H25">
-        <f t="shared" ref="H25" si="2">G25/$K$1*$L$1-$M$1</f>
+        <f t="shared" ref="H25" si="3">G25/$K$1*$L$1-$M$1</f>
         <v>90.462962962962962</v>
       </c>
     </row>

</xml_diff>